<commit_message>
Update Modelo lógico Paciente.xlsx
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Pacientes/Modelo lógico Paciente.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Pacientes/Modelo lógico Paciente.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GOInterop\git\HSL-IPS\Entregaveis\1.RepositorioSemantico\Paciente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Pacientes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABCF94B-243C-411C-80D6-2034D2F50A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10063EBA-5BE5-6545-8D4D-E4C4510C160E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapa semântico" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>Mapeamento semântico</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>https://rnds-fhir.saude.gov.br/ValueSet/BRSexo-1.0</t>
+  </si>
+  <si>
+    <t>http://www.saude.gov.br/fhir/r4/ValueSet/BRRacaCor-1.0</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>https://ips.saude.gov.br/ValueSet/raca-br-ips</t>
+  </si>
+  <si>
+    <t>Não precisa ConceptMap - feita a tradução para Ingles no CodeSystem e carregado na collection</t>
+  </si>
+  <si>
+    <t>sexoNascimento</t>
+  </si>
+  <si>
+    <t>https://ips.saude.gov.br/ValueSet/sexo-nascimento-br-ips</t>
   </si>
 </sst>
 </file>
@@ -329,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -378,23 +396,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -721,24 +729,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -751,8 +759,8 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
@@ -762,15 +770,15 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -789,61 +797,61 @@
       <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25" t="s">
+      <c r="H3" s="22"/>
+      <c r="I3" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="17" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="9"/>
       <c r="B4" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="21" t="b">
+      <c r="F4" s="20" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H4" s="12"/>
+      <c r="I4" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="9"/>
       <c r="B5" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="20" t="b">
+      <c r="F5" s="10" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I5" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="15" t="b">
         <v>1</v>
@@ -866,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="9"/>
       <c r="B7" s="15" t="b">
         <v>1</v>
@@ -889,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="9"/>
       <c r="B8" s="15" t="b">
         <v>1</v>
@@ -912,35 +920,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="9"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
       <c r="B10" s="15" t="b">
         <v>1</v>
       </c>
@@ -948,115 +950,121 @@
         <v>12</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
+      <c r="G10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="13"/>
       <c r="I10" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="9"/>
       <c r="B11" s="15" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="11"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="B12" s="15" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="I12" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="F13" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="G13" s="22" t="s">
-        <v>31</v>
-      </c>
+      <c r="G13" s="11"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="11"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="15" t="b">
         <v>0</v>
@@ -1065,21 +1073,23 @@
         <v>29</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F15" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="15" t="b">
         <v>0</v>
@@ -1088,7 +1098,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>13</v>
@@ -1096,13 +1106,13 @@
       <c r="F16" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="15" t="b">
         <v>0</v>
@@ -1111,21 +1121,21 @@
         <v>29</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="10" t="b">
         <v>0</v>
       </c>
       <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="13"/>
       <c r="I17" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="15" t="b">
         <v>0</v>
@@ -1134,13 +1144,13 @@
         <v>29</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="12"/>
@@ -1148,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
       <c r="B19" s="15" t="b">
         <v>0</v>
@@ -1157,28 +1167,76 @@
         <v>29</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="9"/>
+      <c r="B20" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A21" s="9"/>
+      <c r="B21" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13" t="b">
+      <c r="E21" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1" xr:uid="{0AD04B43-F649-4164-9D31-0893ADD9EB5D}"/>
-    <hyperlink ref="G13" r:id="rId2" xr:uid="{19116853-4923-40E1-92D3-18DB948FC12A}"/>
-    <hyperlink ref="A9" r:id="rId3" xr:uid="{C61F0C2B-FBC7-42E1-BCFE-910D9376FF9B}"/>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{0AD04B43-F649-4164-9D31-0893ADD9EB5D}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{19116853-4923-40E1-92D3-18DB948FC12A}"/>
+    <hyperlink ref="A10" r:id="rId3" xr:uid="{C61F0C2B-FBC7-42E1-BCFE-910D9376FF9B}"/>
+    <hyperlink ref="G12" r:id="rId4" xr:uid="{5F649D52-688C-014F-8C7E-1C8DEB4F9EA6}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{E3430A29-1D23-4B49-8C3E-4B244730292E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>